<commit_message>
corrected links to xlsx files
</commit_message>
<xml_diff>
--- a/topic02/book-c/archives/Solver-Add-In.xlsx
+++ b/topic02/book-c/archives/Solver-Add-In.xlsx
@@ -5,17 +5,17 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmullally\Dropbox\Teaching\2016-2017\Sm2\dataAnalytics\coursera\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmullally\Documents\Analytics\analytics-2017\topic02\book-c\archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Solver - Template" sheetId="1" r:id="rId1"/>
-    <sheet name="Basic Solver - Solution" sheetId="3" r:id="rId2"/>
+    <sheet name="Basic Solver - Solution" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="Solver Challenge - Template" sheetId="2" r:id="rId3"/>
-    <sheet name="Solver Challenge - Solution" sheetId="4" r:id="rId4"/>
+    <sheet name="Solver Challenge - Solution" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Basic Solver - Solution'!$C$4</definedName>
@@ -263,18 +263,21 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -683,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -873,7 +876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1290,7 +1293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>

</xml_diff>